<commit_message>
MVP of status writer
</commit_message>
<xml_diff>
--- a/backend/zTEMPLATE/Finance Documents/newEstimate.xlsx
+++ b/backend/zTEMPLATE/Finance Documents/newEstimate.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="52">
   <si>
     <r>
       <t xml:space="preserve">SAATCHI &amp; SAATCHI </t>
@@ -84,13 +84,31 @@
     <t>LENGTHS</t>
   </si>
   <si>
+    <t>TYFK4241H</t>
+  </si>
+  <si>
+    <t>REV DEC 24 KSC NFL THON P1 SHAKE UP THE HOLIDAYS RAV4 LEASE 1203</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>TYFK4242H</t>
+  </si>
+  <si>
+    <t>REV DEC 24 KSC NFL THON P1 ORNAMENTS RAV4 LEASE 2703</t>
+  </si>
+  <si>
+    <t>TYFK4243H</t>
+  </si>
+  <si>
+    <t>REV DEC 24 KSC NFL THON P1 ORNAMENTS TUNDRA APR 1203</t>
+  </si>
+  <si>
     <t>TYFK4244H</t>
   </si>
   <si>
-    <t>REV DEC ‘24 KSC NFL THON P1 SHAKE UP THE HOLIDAYS TACOMA LEASE OR TUNDRA LEASE 2703</t>
-  </si>
-  <si>
-    <t>unknown</t>
+    <t>REV DEC 24 KSC NFL THON P1 SHAKE UP THE HOLIDAYS TACOMA LEASE OR TUNDRA LEASE 2703</t>
   </si>
   <si>
     <t xml:space="preserve">WORK CATEGORY </t>
@@ -989,37 +1007,55 @@
       <c r="A14">
         <v>2</v>
       </c>
-      <c r="B14" s="22"/>
-      <c r="C14" s="29"/>
+      <c r="B14" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>21</v>
+      </c>
       <c r="D14" s="29"/>
       <c r="E14" s="29"/>
       <c r="F14" s="30"/>
       <c r="G14" s="31"/>
-      <c r="H14" s="32"/>
+      <c r="H14" s="32" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="29"/>
+      <c r="B15" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>23</v>
+      </c>
       <c r="D15" s="29"/>
       <c r="E15" s="29"/>
       <c r="F15" s="30"/>
       <c r="G15" s="31"/>
-      <c r="H15" s="32"/>
+      <c r="H15" s="32" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="29"/>
+      <c r="B16" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>25</v>
+      </c>
       <c r="D16" s="29"/>
       <c r="E16" s="29"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="32"/>
+      <c r="H16" s="32" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
@@ -1127,17 +1163,17 @@
     </row>
     <row r="26" ht="33" customHeight="1" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" s="34" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C26" s="35"/>
       <c r="D26" s="36" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E26" s="36"/>
       <c r="F26" s="36"/>
       <c r="G26" s="37"/>
       <c r="H26" s="38" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="I26" s="37"/>
       <c r="J26" s="37"/>
@@ -1152,11 +1188,11 @@
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" s="40" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="C28" s="18"/>
       <c r="D28" s="41" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E28" s="41"/>
       <c r="F28" s="41"/>
@@ -1168,11 +1204,11 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="40" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C29" s="18"/>
       <c r="D29" s="41" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E29" s="41"/>
       <c r="F29" s="41"/>
@@ -1184,11 +1220,11 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="40" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C30" s="18"/>
       <c r="D30" s="41" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
@@ -1200,11 +1236,11 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" s="40" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C31" s="18"/>
       <c r="D31" s="41" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
@@ -1216,11 +1252,11 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" s="40" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C32" s="18"/>
       <c r="D32" s="41" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
@@ -1232,11 +1268,11 @@
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="40" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="41" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E33" s="41"/>
       <c r="F33" s="41"/>
@@ -1248,11 +1284,11 @@
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="40" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="C34" s="18"/>
       <c r="D34" s="41" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E34" s="41"/>
       <c r="F34" s="41"/>
@@ -1264,11 +1300,11 @@
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" s="40" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="C35" s="18"/>
       <c r="D35" s="41" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E35" s="41"/>
       <c r="F35" s="41"/>
@@ -1280,11 +1316,11 @@
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" s="40" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="41" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E36" s="41"/>
       <c r="F36" s="41"/>
@@ -1310,7 +1346,7 @@
       <c r="B38" s="17"/>
       <c r="C38" s="18"/>
       <c r="D38" s="41" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
@@ -1349,7 +1385,7 @@
       <c r="B40" s="17"/>
       <c r="C40" s="18"/>
       <c r="D40" s="41" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
@@ -1373,7 +1409,7 @@
     </row>
     <row r="42" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D42" s="41" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E42" s="41"/>
       <c r="F42" s="41"/>
@@ -1408,7 +1444,7 @@
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="46" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
@@ -1474,7 +1510,7 @@
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="50"/>
       <c r="C50" s="53" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="D50" s="51"/>
       <c r="E50" s="51"/>

</xml_diff>